<commit_message>
Minor update, corrected input data
</commit_message>
<xml_diff>
--- a/algebras.xlsx
+++ b/algebras.xlsx
@@ -555,6 +555,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -655,10 +656,10 @@
   <dimension ref="A1:J161"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A117" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A146" activeCellId="0" sqref="146:146"/>
+      <selection pane="topLeft" activeCell="A125" activeCellId="0" sqref="125:125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.74"/>
@@ -4761,7 +4762,7 @@
         <v>136</v>
       </c>
       <c r="C125" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>11</v>
@@ -4770,10 +4771,10 @@
         <v>12</v>
       </c>
       <c r="F125" s="2" t="n">
-        <v>50838</v>
+        <v>7252</v>
       </c>
       <c r="G125" s="2" t="n">
-        <v>1179604</v>
+        <v>100506</v>
       </c>
       <c r="H125" s="3" t="n">
         <v>-1</v>

</xml_diff>

<commit_message>
updated scripts for auto-run of experiments
</commit_message>
<xml_diff>
--- a/algebras.xlsx
+++ b/algebras.xlsx
@@ -655,11 +655,11 @@
   </sheetPr>
   <dimension ref="A1:J161"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A117" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A125" activeCellId="0" sqref="125:125"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N20" activeCellId="0" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.74"/>
@@ -1099,7 +1099,7 @@
         <v>24</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>11</v>
@@ -1108,10 +1108,10 @@
         <v>12</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>3589418</v>
+        <v>8272</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>3589418</v>
+        <v>8272</v>
       </c>
       <c r="H14" s="3" t="n">
         <v>-1</v>
@@ -1132,7 +1132,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>11</v>
@@ -1141,10 +1141,10 @@
         <v>12</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>729866</v>
+        <v>8806</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>1156780</v>
+        <v>30274</v>
       </c>
       <c r="H15" s="3" t="n">
         <v>-1</v>
@@ -1198,7 +1198,7 @@
         <v>27</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>11</v>
@@ -1210,7 +1210,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>362880</v>
+        <v>40320</v>
       </c>
       <c r="H17" s="3" t="n">
         <v>-1</v>

</xml_diff>